<commit_message>
system 1 and sha1 access
added login and logout processes for sha1 and system1
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -586,12 +586,10 @@
       <c r="A6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1601,7 +1599,7 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Data Table workflow extraction
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -128,10 +128,13 @@
     <t>System1_Credential</t>
   </si>
   <si>
-    <t>Credential</t>
+    <t>https://acme-test.uipath.com/account/login</t>
   </si>
   <si>
-    <t>https://acme-test.uipath.com/account/login</t>
+    <t>http://www.sha1-online.com/</t>
+  </si>
+  <si>
+    <t>leespino@amazon.com;FE0B8v</t>
   </si>
 </sst>
 </file>
@@ -587,7 +590,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -596,8 +599,8 @@
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="s">
-        <v>27</v>
+      <c r="B8" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -605,8 +608,8 @@
       <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="s">
-        <v>34</v>
+      <c r="B10" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1600,9 +1603,11 @@
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Test Version - Passed
Processed the latest changes to how data is assigned to be then eventually processed. Debugged it and is currently working with IE without any further errors
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -128,13 +128,10 @@
     <t>System1_Credential</t>
   </si>
   <si>
-    <t>https://acme-test.uipath.com/account/login</t>
-  </si>
-  <si>
     <t>http://www.sha1-online.com/</t>
   </si>
   <si>
-    <t>leespino@amazon.com;FE0B8v</t>
+    <t>https://acme-test.uipath.com/</t>
   </si>
 </sst>
 </file>
@@ -516,7 +513,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -590,7 +587,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -600,7 +597,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -609,7 +606,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1602,12 +1599,11 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B8" r:id="rId2"/>
-    <hyperlink ref="B10" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
last commit before grade
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -512,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1611,8 +1611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1663,7 +1663,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>

</xml_diff>